<commit_message>
Deployed 5c2770b with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/eDNA 12S metab/example_output/Biodiversity.xlsx
+++ b/eDNA 12S metab/example_output/Biodiversity.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -382,769 +382,753 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>TDL_EC_49_12S</t>
+          <t>TDL_FS_10_12S</t>
         </is>
       </c>
       <c r="B2">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="C2">
-        <v>2.599</v>
+        <v>0.65</v>
       </c>
       <c r="D2">
-        <v>0.888</v>
+        <v>0.314</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>TDL_FS_10_12S</t>
+          <t>TDL_FS_11_12S</t>
         </is>
       </c>
       <c r="B3">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C3">
-        <v>0.6830000000000001</v>
+        <v>0.843</v>
       </c>
       <c r="D3">
-        <v>0.322</v>
+        <v>0.482</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>TDL_FS_11_12S</t>
+          <t>TDL_FS_12_12S</t>
         </is>
       </c>
       <c r="B4">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>0.873</v>
+        <v>0.478</v>
       </c>
       <c r="D4">
-        <v>0.487</v>
+        <v>0.235</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>TDL_FS_12_12S</t>
+          <t>TDL_FS_14_12S</t>
         </is>
       </c>
       <c r="B5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C5">
-        <v>0.491</v>
+        <v>0.988</v>
       </c>
       <c r="D5">
-        <v>0.238</v>
+        <v>0.458</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>TDL_FS_14_12S</t>
+          <t>TDL_FS_15_12S</t>
         </is>
       </c>
       <c r="B6">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C6">
-        <v>1.277</v>
+        <v>0.894</v>
       </c>
       <c r="D6">
-        <v>0.543</v>
+        <v>0.475</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>TDL_FS_15_12S</t>
+          <t>TDL_FS_16_12S</t>
         </is>
       </c>
       <c r="B7">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="C7">
-        <v>1.21</v>
+        <v>0.551</v>
       </c>
       <c r="D7">
-        <v>0.553</v>
+        <v>0.276</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>TDL_FS_16_12S</t>
+          <t>TDL_FS_17_12S</t>
         </is>
       </c>
       <c r="B8">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C8">
-        <v>0.677</v>
+        <v>0.147</v>
       </c>
       <c r="D8">
-        <v>0.314</v>
+        <v>0.044</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>TDL_FS_17_12S</t>
+          <t>TDL_FS_18_12S</t>
         </is>
       </c>
       <c r="B9">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C9">
-        <v>0.323</v>
+        <v>0.603</v>
       </c>
       <c r="D9">
-        <v>0.101</v>
+        <v>0.211</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>TDL_FS_18_12S</t>
+          <t>TDL_FS_19_12S</t>
         </is>
       </c>
       <c r="B10">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C10">
-        <v>0.736</v>
+        <v>1.934</v>
       </c>
       <c r="D10">
-        <v>0.256</v>
+        <v>0.769</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>TDL_FS_19_12S</t>
+          <t>TDL_FS_1_12S</t>
         </is>
       </c>
       <c r="B11">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C11">
-        <v>2.303</v>
+        <v>1.465</v>
       </c>
       <c r="D11">
-        <v>0.851</v>
+        <v>0.641</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>TDL_FS_1_12S</t>
+          <t>TDL_FS_20_12S</t>
         </is>
       </c>
       <c r="B12">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C12">
-        <v>1.612</v>
+        <v>2.162</v>
       </c>
       <c r="D12">
-        <v>0.706</v>
+        <v>0.8110000000000001</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>TDL_FS_20_12S</t>
+          <t>TDL_FS_21_12S</t>
         </is>
       </c>
       <c r="B13">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C13">
-        <v>2.51</v>
+        <v>2.315</v>
       </c>
       <c r="D13">
-        <v>0.876</v>
+        <v>0.857</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>TDL_FS_21_12S</t>
+          <t>TDL_FS_22_12S</t>
         </is>
       </c>
       <c r="B14">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="C14">
-        <v>2.548</v>
+        <v>1.837</v>
       </c>
       <c r="D14">
-        <v>0.888</v>
+        <v>0.746</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>TDL_FS_22_12S</t>
+          <t>TDL_FS_23_12S</t>
         </is>
       </c>
       <c r="B15">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C15">
-        <v>1.986</v>
+        <v>2.124</v>
       </c>
       <c r="D15">
-        <v>0.768</v>
+        <v>0.839</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>TDL_FS_23_12S</t>
+          <t>TDL_FS_24_12S</t>
         </is>
       </c>
       <c r="B16">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C16">
-        <v>2.487</v>
+        <v>1.863</v>
       </c>
       <c r="D16">
-        <v>0.89</v>
+        <v>0.786</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>TDL_FS_24_12S</t>
+          <t>TDL_FS_25_12S</t>
         </is>
       </c>
       <c r="B17">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C17">
-        <v>2.327</v>
+        <v>1.666</v>
       </c>
       <c r="D17">
-        <v>0.866</v>
+        <v>0.735</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>TDL_FS_25_12S</t>
+          <t>TDL_FS_26_12S</t>
         </is>
       </c>
       <c r="B18">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C18">
-        <v>1.789</v>
+        <v>1.386</v>
       </c>
       <c r="D18">
-        <v>0.753</v>
+        <v>0.633</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>TDL_FS_26_12S</t>
+          <t>TDL_FS_27_12S</t>
         </is>
       </c>
       <c r="B19">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C19">
-        <v>1.727</v>
+        <v>1.544</v>
       </c>
       <c r="D19">
-        <v>0.705</v>
+        <v>0.709</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>TDL_FS_27_12S</t>
+          <t>TDL_FS_28_12S</t>
         </is>
       </c>
       <c r="B20">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C20">
-        <v>1.628</v>
+        <v>1.86</v>
       </c>
       <c r="D20">
-        <v>0.723</v>
+        <v>0.784</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>TDL_FS_28_12S</t>
+          <t>TDL_FS_29_12S</t>
         </is>
       </c>
       <c r="B21">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="C21">
-        <v>2.157</v>
+        <v>1.724</v>
       </c>
       <c r="D21">
-        <v>0.826</v>
+        <v>0.746</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>TDL_FS_29_12S</t>
+          <t>TDL_FS_2_12S</t>
         </is>
       </c>
       <c r="B22">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C22">
-        <v>1.796</v>
+        <v>1.553</v>
       </c>
       <c r="D22">
-        <v>0.757</v>
+        <v>0.709</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>TDL_FS_2_12S</t>
+          <t>TDL_FS_30_12S</t>
         </is>
       </c>
       <c r="B23">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C23">
-        <v>1.806</v>
+        <v>1.669</v>
       </c>
       <c r="D23">
-        <v>0.746</v>
+        <v>0.757</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>TDL_FS_30_12S</t>
+          <t>TDL_FS_31_12S</t>
         </is>
       </c>
       <c r="B24">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C24">
-        <v>1.885</v>
+        <v>2.104</v>
       </c>
       <c r="D24">
-        <v>0.784</v>
+        <v>0.8149999999999999</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>TDL_FS_31_12S</t>
+          <t>TDL_FS_32_12S</t>
         </is>
       </c>
       <c r="B25">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C25">
-        <v>2.412</v>
+        <v>0.773</v>
       </c>
       <c r="D25">
-        <v>0.853</v>
+        <v>0.294</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>TDL_FS_32_12S</t>
+          <t>TDL_FS_33_12S</t>
         </is>
       </c>
       <c r="B26">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C26">
-        <v>1.156</v>
+        <v>1.888</v>
       </c>
       <c r="D26">
-        <v>0.408</v>
+        <v>0.722</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>TDL_FS_33_12S</t>
+          <t>TDL_FS_34_12S</t>
         </is>
       </c>
       <c r="B27">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C27">
-        <v>2.406</v>
+        <v>1.714</v>
       </c>
       <c r="D27">
-        <v>0.837</v>
+        <v>0.728</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>TDL_FS_34_12S</t>
+          <t>TDL_FS_35_12S</t>
         </is>
       </c>
       <c r="B28">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28">
-        <v>1.903</v>
+        <v>1.25</v>
       </c>
       <c r="D28">
-        <v>0.753</v>
+        <v>0.544</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>TDL_FS_35_12S</t>
+          <t>TDL_FS_36_12S</t>
         </is>
       </c>
       <c r="B29">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="C29">
-        <v>1.673</v>
+        <v>1.613</v>
       </c>
       <c r="D29">
-        <v>0.633</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>TDL_FS_36_12S</t>
+          <t>TDL_FS_37_12S</t>
         </is>
       </c>
       <c r="B30">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C30">
-        <v>1.903</v>
+        <v>1.938</v>
       </c>
       <c r="D30">
-        <v>0.777</v>
+        <v>0.738</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>TDL_FS_37_12S</t>
+          <t>TDL_FS_38_12S</t>
         </is>
       </c>
       <c r="B31">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C31">
-        <v>2.342</v>
+        <v>2.034</v>
       </c>
       <c r="D31">
-        <v>0.8169999999999999</v>
+        <v>0.751</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>TDL_FS_38_12S</t>
+          <t>TDL_FS_39_12S</t>
         </is>
       </c>
       <c r="B32">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C32">
-        <v>2.394</v>
+        <v>1.989</v>
       </c>
       <c r="D32">
-        <v>0.8159999999999999</v>
+        <v>0.744</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>TDL_FS_39_12S</t>
+          <t>TDL_FS_3_12S</t>
         </is>
       </c>
       <c r="B33">
-        <v>58</v>
+        <v>16</v>
       </c>
       <c r="C33">
-        <v>2.594</v>
+        <v>1.182</v>
       </c>
       <c r="D33">
-        <v>0.885</v>
+        <v>0.544</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>TDL_FS_3_12S</t>
+          <t>TDL_FS_40_12S</t>
         </is>
       </c>
       <c r="B34">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C34">
-        <v>1.279</v>
+        <v>1.938</v>
       </c>
       <c r="D34">
-        <v>0.5659999999999999</v>
+        <v>0.785</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>TDL_FS_40_12S</t>
+          <t>TDL_FS_41_12S</t>
         </is>
       </c>
       <c r="B35">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="C35">
-        <v>2.302</v>
+        <v>1.68</v>
       </c>
       <c r="D35">
-        <v>0.847</v>
+        <v>0.719</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>TDL_FS_41_12S</t>
+          <t>TDL_FS_42_12S</t>
         </is>
       </c>
       <c r="B36">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C36">
-        <v>1.971</v>
+        <v>2.077</v>
       </c>
       <c r="D36">
-        <v>0.785</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>TDL_FS_42_12S</t>
+          <t>TDL_FS_43_12S</t>
         </is>
       </c>
       <c r="B37">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="C37">
-        <v>2.377</v>
+        <v>1.853</v>
       </c>
       <c r="D37">
-        <v>0.845</v>
+        <v>0.759</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>TDL_FS_43_12S</t>
+          <t>TDL_FS_44_12S</t>
         </is>
       </c>
       <c r="B38">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C38">
-        <v>2.245</v>
+        <v>1.706</v>
       </c>
       <c r="D38">
-        <v>0.834</v>
+        <v>0.723</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>TDL_FS_44_12S</t>
+          <t>TDL_FS_45_12S</t>
         </is>
       </c>
       <c r="B39">
         <v>25</v>
       </c>
       <c r="C39">
-        <v>1.976</v>
+        <v>1.715</v>
       </c>
       <c r="D39">
-        <v>0.773</v>
+        <v>0.732</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>TDL_FS_45_12S</t>
+          <t>TDL_FS_46_12S</t>
         </is>
       </c>
       <c r="B40">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C40">
-        <v>1.978</v>
+        <v>1.299</v>
       </c>
       <c r="D40">
-        <v>0.78</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>TDL_FS_46_12S</t>
+          <t>TDL_FS_47_12S</t>
         </is>
       </c>
       <c r="B41">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="C41">
-        <v>1.854</v>
+        <v>2.306</v>
       </c>
       <c r="D41">
-        <v>0.729</v>
+        <v>0.779</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>TDL_FS_47_12S</t>
+          <t>TDL_FS_48_12S</t>
         </is>
       </c>
       <c r="B42">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="C42">
-        <v>2.676</v>
+        <v>2.612</v>
       </c>
       <c r="D42">
-        <v>0.892</v>
+        <v>0.885</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>TDL_FS_48_12S</t>
+          <t>TDL_FS_4_12S</t>
         </is>
       </c>
       <c r="B43">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="C43">
-        <v>2.874</v>
+        <v>1.118</v>
       </c>
       <c r="D43">
-        <v>0.921</v>
+        <v>0.511</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>TDL_FS_4_12S</t>
+          <t>TDL_FS_5_12S</t>
         </is>
       </c>
       <c r="B44">
         <v>16</v>
       </c>
       <c r="C44">
-        <v>1.274</v>
+        <v>1.014</v>
       </c>
       <c r="D44">
-        <v>0.549</v>
+        <v>0.435</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>TDL_FS_5_12S</t>
+          <t>TDL_FS_6_12S</t>
         </is>
       </c>
       <c r="B45">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C45">
-        <v>1.215</v>
+        <v>0.432</v>
       </c>
       <c r="D45">
-        <v>0.495</v>
+        <v>0.178</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>TDL_FS_6_12S</t>
+          <t>TDL_FS_7_12S</t>
         </is>
       </c>
       <c r="B46">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C46">
-        <v>0.476</v>
+        <v>0.534</v>
       </c>
       <c r="D46">
-        <v>0.19</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>TDL_FS_7_12S</t>
+          <t>TDL_FS_8_12S</t>
         </is>
       </c>
       <c r="B47">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C47">
-        <v>0.609</v>
+        <v>0.851</v>
       </c>
       <c r="D47">
-        <v>0.258</v>
+        <v>0.527</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>TDL_FS_8_12S</t>
+          <t>TDL_FS_9_12S</t>
         </is>
       </c>
       <c r="B48">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C48">
-        <v>0.976</v>
+        <v>1.256</v>
       </c>
       <c r="D48">
-        <v>0.552</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>TDL_FS_9_12S</t>
-        </is>
-      </c>
-      <c r="B49">
-        <v>19</v>
-      </c>
-      <c r="C49">
-        <v>1.276</v>
-      </c>
-      <c r="D49">
-        <v>0.673</v>
+        <v>0.671</v>
       </c>
     </row>
   </sheetData>

</xml_diff>